<commit_message>
Add for 5 referee
</commit_message>
<xml_diff>
--- a/src/assets/template/1-Mau_Chuan_Doi_Khang.xlsx
+++ b/src/assets/template/1-Mau_Chuan_Doi_Khang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Project\cocvuong-react\ref\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Project\cocvuong.com\src\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89207FE-21CF-4F1B-B018-75ECD1E677EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027A6DF3-DA5B-4551-ACF5-649C2176D6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-5460" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="13" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="137">
   <si>
     <t>Nguyễn Thành Nhân</t>
   </si>
@@ -402,10 +402,43 @@
     <t>CODE/ĐƠN VỊ GIÁP XANH</t>
   </si>
   <si>
-    <t>QUỐC GIA</t>
-  </si>
-  <si>
     <t>VN</t>
+  </si>
+  <si>
+    <t>QUỐC GIA ĐỎ</t>
+  </si>
+  <si>
+    <t>QUỐC GIA XANH</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>KH</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>MY</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>TL</t>
   </si>
 </sst>
 </file>
@@ -790,10 +823,10 @@
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -813,7 +846,7 @@
         <v>121</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>122</v>
@@ -822,7 +855,7 @@
         <v>123</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -842,13 +875,13 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -868,7 +901,7 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -877,7 +910,7 @@
         <v>9</v>
       </c>
       <c r="I3" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -897,7 +930,7 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -906,7 +939,7 @@
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -926,7 +959,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -935,7 +968,7 @@
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -955,7 +988,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
@@ -964,7 +997,7 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -984,7 +1017,7 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
@@ -993,7 +1026,7 @@
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1013,7 +1046,7 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G8" t="s">
         <v>22</v>
@@ -1022,7 +1055,7 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1038,9 +1071,6 @@
       <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" t="s">
-        <v>125</v>
-      </c>
       <c r="G9" t="s">
         <v>24</v>
       </c>
@@ -1048,7 +1078,7 @@
         <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1068,13 +1098,10 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G10" t="s">
         <v>26</v>
-      </c>
-      <c r="I10" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1090,9 +1117,6 @@
       <c r="D11" t="s">
         <v>27</v>
       </c>
-      <c r="F11" t="s">
-        <v>125</v>
-      </c>
       <c r="G11" t="s">
         <v>28</v>
       </c>
@@ -1100,7 +1124,7 @@
         <v>4</v>
       </c>
       <c r="I11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1120,7 +1144,7 @@
         <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G12" t="s">
         <v>31</v>
@@ -1129,7 +1153,7 @@
         <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1145,9 +1169,6 @@
       <c r="D13" t="s">
         <v>32</v>
       </c>
-      <c r="F13" t="s">
-        <v>125</v>
-      </c>
       <c r="G13" t="s">
         <v>33</v>
       </c>
@@ -1155,7 +1176,7 @@
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1175,13 +1196,10 @@
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G14" t="s">
         <v>35</v>
-      </c>
-      <c r="I14" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1201,7 +1219,7 @@
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G15" t="s">
         <v>37</v>
@@ -1210,7 +1228,7 @@
         <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1230,7 +1248,7 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G16" t="s">
         <v>40</v>
@@ -1239,7 +1257,7 @@
         <v>4</v>
       </c>
       <c r="I16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1259,7 +1277,7 @@
         <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G17" t="s">
         <v>42</v>
@@ -1268,7 +1286,7 @@
         <v>6</v>
       </c>
       <c r="I17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1288,7 +1306,7 @@
         <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G18" t="s">
         <v>44</v>
@@ -1297,7 +1315,7 @@
         <v>9</v>
       </c>
       <c r="I18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1317,7 +1335,7 @@
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G19" t="s">
         <v>47</v>
@@ -1326,7 +1344,7 @@
         <v>6</v>
       </c>
       <c r="I19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1346,7 +1364,7 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G20" t="s">
         <v>0</v>
@@ -1355,7 +1373,7 @@
         <v>4</v>
       </c>
       <c r="I20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1375,7 +1393,7 @@
         <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G21" t="s">
         <v>50</v>
@@ -1384,7 +1402,7 @@
         <v>4</v>
       </c>
       <c r="I21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1404,7 +1422,7 @@
         <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G22" t="s">
         <v>52</v>
@@ -1413,7 +1431,7 @@
         <v>4</v>
       </c>
       <c r="I22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1433,7 +1451,7 @@
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G23" t="s">
         <v>55</v>
@@ -1442,7 +1460,7 @@
         <v>19</v>
       </c>
       <c r="I23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1462,7 +1480,7 @@
         <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G24" t="s">
         <v>57</v>
@@ -1471,7 +1489,7 @@
         <v>6</v>
       </c>
       <c r="I24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1491,7 +1509,7 @@
         <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G25" t="s">
         <v>61</v>
@@ -1500,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="I25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1520,7 +1538,7 @@
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G26" t="s">
         <v>63</v>
@@ -1529,7 +1547,7 @@
         <v>6</v>
       </c>
       <c r="I26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1545,9 +1563,6 @@
       <c r="D27" t="s">
         <v>64</v>
       </c>
-      <c r="F27" t="s">
-        <v>125</v>
-      </c>
       <c r="G27" t="s">
         <v>65</v>
       </c>
@@ -1555,7 +1570,7 @@
         <v>9</v>
       </c>
       <c r="I27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1575,7 +1590,7 @@
         <v>6</v>
       </c>
       <c r="F28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G28" t="s">
         <v>68</v>
@@ -1584,7 +1599,7 @@
         <v>19</v>
       </c>
       <c r="I28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1604,7 +1619,7 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G29" t="s">
         <v>71</v>
@@ -1613,7 +1628,7 @@
         <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1629,14 +1644,8 @@
       <c r="D30" t="s">
         <v>72</v>
       </c>
-      <c r="F30" t="s">
-        <v>125</v>
-      </c>
       <c r="G30" t="s">
         <v>73</v>
-      </c>
-      <c r="I30" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1652,14 +1661,8 @@
       <c r="D31" t="s">
         <v>74</v>
       </c>
-      <c r="F31" t="s">
-        <v>125</v>
-      </c>
       <c r="G31" t="s">
         <v>75</v>
-      </c>
-      <c r="I31" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1675,14 +1678,8 @@
       <c r="D32" t="s">
         <v>76</v>
       </c>
-      <c r="F32" t="s">
-        <v>125</v>
-      </c>
       <c r="G32" t="s">
         <v>77</v>
-      </c>
-      <c r="I32" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1698,14 +1695,8 @@
       <c r="D33" t="s">
         <v>78</v>
       </c>
-      <c r="F33" t="s">
-        <v>125</v>
-      </c>
       <c r="G33" t="s">
         <v>79</v>
-      </c>
-      <c r="I33" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1725,13 +1716,10 @@
         <v>4</v>
       </c>
       <c r="F34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G34" t="s">
         <v>81</v>
-      </c>
-      <c r="I34" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1747,14 +1735,8 @@
       <c r="D35" t="s">
         <v>82</v>
       </c>
-      <c r="F35" t="s">
-        <v>125</v>
-      </c>
       <c r="G35" t="s">
         <v>83</v>
-      </c>
-      <c r="I35" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1770,14 +1752,8 @@
       <c r="D36" t="s">
         <v>84</v>
       </c>
-      <c r="F36" t="s">
-        <v>125</v>
-      </c>
       <c r="G36" t="s">
         <v>85</v>
-      </c>
-      <c r="I36" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1793,14 +1769,8 @@
       <c r="D37" t="s">
         <v>86</v>
       </c>
-      <c r="F37" t="s">
-        <v>125</v>
-      </c>
       <c r="G37" t="s">
         <v>87</v>
-      </c>
-      <c r="I37" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1820,13 +1790,10 @@
         <v>19</v>
       </c>
       <c r="F38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G38" t="s">
         <v>89</v>
-      </c>
-      <c r="I38" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1842,9 +1809,6 @@
       <c r="D39" t="s">
         <v>90</v>
       </c>
-      <c r="F39" t="s">
-        <v>125</v>
-      </c>
       <c r="G39" t="s">
         <v>91</v>
       </c>
@@ -1852,7 +1816,7 @@
         <v>9</v>
       </c>
       <c r="I39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1872,13 +1836,10 @@
         <v>19</v>
       </c>
       <c r="F40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G40" t="s">
         <v>94</v>
-      </c>
-      <c r="I40" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1894,14 +1855,8 @@
       <c r="D41" t="s">
         <v>95</v>
       </c>
-      <c r="F41" t="s">
-        <v>125</v>
-      </c>
       <c r="G41" t="s">
         <v>96</v>
-      </c>
-      <c r="I41" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1921,7 +1876,7 @@
         <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G42" t="s">
         <v>99</v>
@@ -1930,7 +1885,7 @@
         <v>4</v>
       </c>
       <c r="I42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1950,13 +1905,10 @@
         <v>4</v>
       </c>
       <c r="F43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G43" t="s">
         <v>101</v>
-      </c>
-      <c r="I43" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -1976,13 +1928,10 @@
         <v>6</v>
       </c>
       <c r="F44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G44" t="s">
         <v>104</v>
-      </c>
-      <c r="I44" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -1998,14 +1947,8 @@
       <c r="D45" t="s">
         <v>105</v>
       </c>
-      <c r="F45" t="s">
-        <v>125</v>
-      </c>
       <c r="G45" t="s">
         <v>106</v>
-      </c>
-      <c r="I45" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2021,14 +1964,8 @@
       <c r="D46" t="s">
         <v>107</v>
       </c>
-      <c r="F46" t="s">
-        <v>125</v>
-      </c>
       <c r="G46" t="s">
         <v>108</v>
-      </c>
-      <c r="I46" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2044,14 +1981,8 @@
       <c r="D47" t="s">
         <v>109</v>
       </c>
-      <c r="F47" t="s">
-        <v>125</v>
-      </c>
       <c r="G47" t="s">
         <v>110</v>
-      </c>
-      <c r="I47" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2067,17 +1998,11 @@
       <c r="D48" t="s">
         <v>111</v>
       </c>
-      <c r="F48" t="s">
-        <v>125</v>
-      </c>
       <c r="G48" t="s">
         <v>112</v>
       </c>
-      <c r="I48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2090,90 +2015,84 @@
       <c r="D49" t="s">
         <v>113</v>
       </c>
-      <c r="F49" t="s">
-        <v>125</v>
-      </c>
       <c r="G49" t="s">
         <v>114</v>
       </c>
       <c r="H49" t="s">
         <v>115</v>
       </c>
-      <c r="I49" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>116</v>
       </c>

</xml_diff>